<commit_message>
added mean decision time per user per alarm analysis. Changed plots to APA7 styling
</commit_message>
<xml_diff>
--- a/excel/cry-wolf_20200125_14-35-09_patched_decision_time.xlsx
+++ b/excel/cry-wolf_20200125_14-35-09_patched_decision_time.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BA53"/>
+  <dimension ref="A1:BA54"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9073,6 +9073,167 @@
         <v>0.0001491982638888889</v>
       </c>
     </row>
+    <row r="54">
+      <c r="A54" s="2" t="n">
+        <v>0.0001670052083333333</v>
+      </c>
+      <c r="B54" s="2" t="n">
+        <v>0.0002745775462962963</v>
+      </c>
+      <c r="C54" s="2" t="n">
+        <v>0.0001460196296296296</v>
+      </c>
+      <c r="D54" s="2" t="n">
+        <v>0.0004084809027777777</v>
+      </c>
+      <c r="E54" s="2" t="n">
+        <v>0.0001808335532407407</v>
+      </c>
+      <c r="F54" s="2" t="n">
+        <v>0.0001735133912037037</v>
+      </c>
+      <c r="G54" s="2" t="n">
+        <v>0.0002188089814814815</v>
+      </c>
+      <c r="H54" s="2" t="n">
+        <v>0.0002625146875</v>
+      </c>
+      <c r="I54" s="2" t="n">
+        <v>0.0002728821643518519</v>
+      </c>
+      <c r="J54" s="2" t="n">
+        <v>0.0001616913657407407</v>
+      </c>
+      <c r="K54" s="2" t="n">
+        <v>0.0002051313194444444</v>
+      </c>
+      <c r="L54" s="2" t="n">
+        <v>0.0001135276388888889</v>
+      </c>
+      <c r="M54" s="2" t="n">
+        <v>0.0001955103703703704</v>
+      </c>
+      <c r="N54" s="2" t="n">
+        <v>0.0001846696875</v>
+      </c>
+      <c r="O54" s="2" t="n">
+        <v>0.0001615680555555556</v>
+      </c>
+      <c r="P54" s="2" t="n">
+        <v>0.0001802319212962963</v>
+      </c>
+      <c r="Q54" s="2" t="n">
+        <v>0.0001749151967592592</v>
+      </c>
+      <c r="R54" s="2" t="n">
+        <v>0.0003599841898148148</v>
+      </c>
+      <c r="S54" s="2" t="n">
+        <v>0.0001567690509259259</v>
+      </c>
+      <c r="T54" s="2" t="n">
+        <v>0.0001685033796296296</v>
+      </c>
+      <c r="U54" s="2" t="n">
+        <v>0.0001635503472222222</v>
+      </c>
+      <c r="V54" s="2" t="n">
+        <v>0.0002061656365740741</v>
+      </c>
+      <c r="W54" s="2" t="n">
+        <v>0.0001455506481481481</v>
+      </c>
+      <c r="X54" s="2" t="n">
+        <v>0.0001440444675925926</v>
+      </c>
+      <c r="Y54" s="2" t="n">
+        <v>0.0001581833101851852</v>
+      </c>
+      <c r="Z54" s="2" t="n">
+        <v>0.0003038575</v>
+      </c>
+      <c r="AA54" s="2" t="n">
+        <v>0.0003003331944444444</v>
+      </c>
+      <c r="AB54" s="2" t="n">
+        <v>0.0002600870254629629</v>
+      </c>
+      <c r="AC54" s="2" t="n">
+        <v>0.0002629990162037037</v>
+      </c>
+      <c r="AD54" s="2" t="n">
+        <v>0.0001660394328703704</v>
+      </c>
+      <c r="AE54" s="2" t="n">
+        <v>0.0002433874189814815</v>
+      </c>
+      <c r="AF54" s="2" t="n">
+        <v>0.0002855700231481481</v>
+      </c>
+      <c r="AG54" s="2" t="n">
+        <v>0.0002022409143518518</v>
+      </c>
+      <c r="AH54" s="2" t="n">
+        <v>0.0001460596875</v>
+      </c>
+      <c r="AI54" s="2" t="n">
+        <v>0.000284883587962963</v>
+      </c>
+      <c r="AJ54" s="2" t="n">
+        <v>0.0002435454398148148</v>
+      </c>
+      <c r="AK54" s="2" t="n">
+        <v>0.0001806169791666667</v>
+      </c>
+      <c r="AL54" s="2" t="n">
+        <v>0.0001690469097222222</v>
+      </c>
+      <c r="AM54" s="2" t="n">
+        <v>9.776553240740741e-05</v>
+      </c>
+      <c r="AN54" s="2" t="n">
+        <v>0.0001444139467592593</v>
+      </c>
+      <c r="AO54" s="2" t="n">
+        <v>0.000265443587962963</v>
+      </c>
+      <c r="AP54" s="2" t="n">
+        <v>0.0003188993402777778</v>
+      </c>
+      <c r="AQ54" s="2" t="n">
+        <v>0.0003747275578703703</v>
+      </c>
+      <c r="AR54" s="2" t="n">
+        <v>0.0002739803587962963</v>
+      </c>
+      <c r="AS54" s="2" t="n">
+        <v>0.0001828854976851852</v>
+      </c>
+      <c r="AT54" s="2" t="n">
+        <v>0.0002432567592592593</v>
+      </c>
+      <c r="AU54" s="2" t="n">
+        <v>0.0002172707407407408</v>
+      </c>
+      <c r="AV54" s="2" t="n">
+        <v>0.0002529148842592593</v>
+      </c>
+      <c r="AW54" s="2" t="n">
+        <v>0.0002858644907407408</v>
+      </c>
+      <c r="AX54" s="2" t="n">
+        <v>0.0001850865740740741</v>
+      </c>
+      <c r="AY54" s="2" t="n">
+        <v>0.0002251333217592593</v>
+      </c>
+      <c r="AZ54" s="2" t="n">
+        <v>0.0001195023148148148</v>
+      </c>
+      <c r="BA54" s="2" t="n">
+        <v>0.0002157777777777778</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>